<commit_message>
new operations and battles
</commit_message>
<xml_diff>
--- a/RedditBattles_Operations.xlsx
+++ b/RedditBattles_Operations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\WW2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\WW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
   <si>
     <t>Battle of Moscow</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Battle (sort of)</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +634,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -639,7 +642,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -647,7 +650,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -655,7 +658,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -663,7 +666,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -671,7 +674,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -679,7 +682,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -687,7 +690,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -695,7 +698,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -703,7 +706,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -711,7 +714,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -719,7 +722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -727,7 +730,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -735,44 +738,59 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Data + styling + Release 19062017
</commit_message>
<xml_diff>
--- a/RedditBattles_Operations.xlsx
+++ b/RedditBattles_Operations.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\WW2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\WW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>Battle of Moscow</t>
   </si>
@@ -501,7 +501,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,6 +529,9 @@
       <c r="B3" t="s">
         <v>34</v>
       </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -537,6 +540,9 @@
       <c r="B4" t="s">
         <v>34</v>
       </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -553,6 +559,9 @@
       <c r="B6" t="s">
         <v>34</v>
       </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -704,6 +713,9 @@
       </c>
       <c r="B25" t="s">
         <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
more battles and divisions
</commit_message>
<xml_diff>
--- a/RedditBattles_Operations.xlsx
+++ b/RedditBattles_Operations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="46">
   <si>
     <t>Battle of Moscow</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>Henry</t>
-  </si>
-  <si>
-    <t>Carina</t>
   </si>
   <si>
     <t>Henry!</t>
@@ -518,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +740,7 @@
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -798,7 +795,7 @@
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -809,7 +806,7 @@
         <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -891,7 +888,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
@@ -902,7 +899,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>

</xml_diff>